<commit_message>
updates schemas and analysis code
</commit_message>
<xml_diff>
--- a/schemas/processingPipelineSchema.xlsx
+++ b/schemas/processingPipelineSchema.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{6F79A314-FB93-4CE0-9B48-700EA16B140B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32E5698D-EECA-4162-8ECB-007C6389A52A}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{6F79A314-FB93-4CE0-9B48-700EA16B140B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F79D74D3-4A3B-42BE-B1C8-138F2FFB421F}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30600" yWindow="-660" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="environmentalSample" sheetId="1" r:id="rId1"/>
     <sheet name="zebrafish raw data" sheetId="2" r:id="rId2"/>
-    <sheet name="zebrafish processed data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="139">
   <si>
     <t>SampleNumber</t>
   </si>
@@ -836,15 +835,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="146" customWidth="1"/>
+    <col min="3" max="3" width="117" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="196.42578125" bestFit="1" customWidth="1"/>
@@ -1421,7 +1420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1581,33 +1580,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>